<commit_message>
fixing facies analysis for publication (in progress)
</commit_message>
<xml_diff>
--- a/data/exp_pro/integration_results_part2.xlsx
+++ b/data/exp_pro/integration_results_part2.xlsx
@@ -583,9 +583,7 @@
       <c r="N2" t="s">
         <v>16</v>
       </c>
-      <c r="O2">
-        <v>1.3</v>
-      </c>
+      <c r="O2"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
@@ -631,7 +629,7 @@
         <v>18</v>
       </c>
       <c r="O3">
-        <v>0.65</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -678,7 +676,7 @@
         <v>18</v>
       </c>
       <c r="O4">
-        <v>2.9</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -725,7 +723,7 @@
         <v>18</v>
       </c>
       <c r="O5">
-        <v>2.06</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -772,7 +770,7 @@
         <v>18</v>
       </c>
       <c r="O6">
-        <v>40.1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -819,7 +817,7 @@
         <v>18</v>
       </c>
       <c r="O7">
-        <v>24.6</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -865,9 +863,7 @@
       <c r="N8" t="s">
         <v>24</v>
       </c>
-      <c r="O8">
-        <v>0.89</v>
-      </c>
+      <c r="O8"/>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
@@ -912,9 +908,7 @@
       <c r="N9" t="s">
         <v>24</v>
       </c>
-      <c r="O9">
-        <v>0.53</v>
-      </c>
+      <c r="O9"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
@@ -960,7 +954,7 @@
         <v>27</v>
       </c>
       <c r="O10">
-        <v>3.49</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1007,7 +1001,7 @@
         <v>27</v>
       </c>
       <c r="O11">
-        <v>29.5</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1054,7 +1048,7 @@
         <v>30</v>
       </c>
       <c r="O12">
-        <v>0.45</v>
+        <v>8.7</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1101,7 +1095,7 @@
         <v>30</v>
       </c>
       <c r="O13">
-        <v>19.6</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1148,7 +1142,7 @@
         <v>30</v>
       </c>
       <c r="O14">
-        <v>20.1</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1194,9 +1188,7 @@
       <c r="N15" t="s">
         <v>24</v>
       </c>
-      <c r="O15">
-        <v>30.8</v>
-      </c>
+      <c r="O15"/>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
@@ -1242,7 +1234,7 @@
         <v>35</v>
       </c>
       <c r="O16">
-        <v>4.9</v>
+        <v>9.2</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1288,9 +1280,7 @@
       <c r="N17" t="s">
         <v>35</v>
       </c>
-      <c r="O17">
-        <v>25.4</v>
-      </c>
+      <c r="O17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
corrected data added a brief sulfur analysis script with stoichiometric ratios for NO₃⁻ and SO₄²⁻ reactions and improved the plots (to be finished).
</commit_message>
<xml_diff>
--- a/data/exp_pro/integration_results_part2.xlsx
+++ b/data/exp_pro/integration_results_part2.xlsx
@@ -583,7 +583,9 @@
       <c r="N2" t="s">
         <v>16</v>
       </c>
-      <c r="O2"/>
+      <c r="O2">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
@@ -817,7 +819,7 @@
         <v>18</v>
       </c>
       <c r="O7">
-        <v>15.4</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -858,7 +860,7 @@
         <v>0.11063051769861963</v>
       </c>
       <c r="M8">
-        <v>3.0100000000000007</v>
+        <v>3.42</v>
       </c>
       <c r="N8" t="s">
         <v>24</v>
@@ -903,12 +905,14 @@
         <v>0.45978569292471283</v>
       </c>
       <c r="M9">
-        <v>3.6100000000000003</v>
+        <v>3.51</v>
       </c>
       <c r="N9" t="s">
         <v>24</v>
       </c>
-      <c r="O9"/>
+      <c r="O9">
+        <v>42.6</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
@@ -954,7 +958,7 @@
         <v>27</v>
       </c>
       <c r="O10">
-        <v>3.7</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1183,12 +1187,14 @@
         <v>0.4281429971149485</v>
       </c>
       <c r="M15">
-        <v>3.51</v>
+        <v>3.34</v>
       </c>
       <c r="N15" t="s">
         <v>24</v>
       </c>
-      <c r="O15"/>
+      <c r="O15">
+        <v>44.0</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
@@ -1280,7 +1286,9 @@
       <c r="N17" t="s">
         <v>35</v>
       </c>
-      <c r="O17"/>
+      <c r="O17">
+        <v>20.05</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>